<commit_message>
Add reference impl experiments
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Projects\Repos\TCP-Forum-Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git Repos\TCP-Forum-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B677FE24-2C10-4996-B2A7-C7341C9D1C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E079548-AFA3-4993-98AB-E57B7B2F672D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9684" yWindow="3516" windowWidth="17280" windowHeight="8964" xr2:uid="{A70D0F38-2F49-4733-A14D-F7656FB5FA56}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A70D0F38-2F49-4733-A14D-F7656FB5FA56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4483,21 +4483,21 @@
       <selection activeCell="D427" sqref="D427"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4520,8 +4520,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>539.18245761523031</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -4563,14 +4563,14 @@
         <v>21543.599999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>19897.099999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -4604,14 +4604,14 @@
         <v>19805.099999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>19571.2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -4645,14 +4645,14 @@
         <v>18554.7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>19613.400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -4686,14 +4686,14 @@
         <v>19539.7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>19687.099999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -4727,14 +4727,14 @@
         <v>19505.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>20000.2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -4768,14 +4768,14 @@
         <v>19927</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>20077.400000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>2</v>
       </c>
@@ -4809,14 +4809,14 @@
         <v>19987.8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>19920.8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
@@ -4850,14 +4850,14 @@
         <v>19770.3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>1</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>20548.599999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>2</v>
       </c>
@@ -4891,14 +4891,14 @@
         <v>20378</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>1</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>20031.2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
@@ -4932,8 +4932,8 @@
         <v>19708.599999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>15798.9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>2</v>
       </c>
@@ -4967,14 +4967,14 @@
         <v>15105.1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>1</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>15780.1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
@@ -5008,14 +5008,14 @@
         <v>15200.6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>1</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>15185.1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>2</v>
       </c>
@@ -5049,14 +5049,14 @@
         <v>14888.7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>1</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>15659.7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>2</v>
       </c>
@@ -5090,14 +5090,14 @@
         <v>15046.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>1</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>15554.5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>2</v>
       </c>
@@ -5131,14 +5131,14 @@
         <v>15235.4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>1</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>15400.5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>2</v>
       </c>
@@ -5172,14 +5172,14 @@
         <v>14625</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>1</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>15684.8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>2</v>
       </c>
@@ -5213,14 +5213,14 @@
         <v>14827.2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>1</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>15611.4</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>2</v>
       </c>
@@ -5254,14 +5254,14 @@
         <v>15114.7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>1</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>15754.8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>2</v>
       </c>
@@ -5295,14 +5295,14 @@
         <v>15199.3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>1</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>15210.3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>2</v>
       </c>
@@ -5336,8 +5336,8 @@
         <v>14786.5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>11104.2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>2</v>
       </c>
@@ -5371,14 +5371,14 @@
         <v>10719.1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>1</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>11120.2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>2</v>
       </c>
@@ -5412,14 +5412,14 @@
         <v>10700.4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>1</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>10990.7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>2</v>
       </c>
@@ -5453,14 +5453,14 @@
         <v>10579.1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="6"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>1</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>10795.9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>2</v>
       </c>
@@ -5494,14 +5494,14 @@
         <v>10513.7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>1</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>10798.7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>2</v>
       </c>
@@ -5535,14 +5535,14 @@
         <v>10458.4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="6"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>1</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>10874.8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>2</v>
       </c>
@@ -5576,14 +5576,14 @@
         <v>10558.7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>1</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>10878.2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>2</v>
       </c>
@@ -5617,14 +5617,14 @@
         <v>10549.4</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>1</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>10821.8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>2</v>
       </c>
@@ -5658,14 +5658,14 @@
         <v>10497.6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>1</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>11353.1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>2</v>
       </c>
@@ -5699,14 +5699,14 @@
         <v>10751.4</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="6"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>1</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>10748.1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>2</v>
       </c>
@@ -5740,8 +5740,8 @@
         <v>10339.299999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>1</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>18079.7</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>2</v>
       </c>
@@ -5775,14 +5775,14 @@
         <v>17801.400000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="6"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>1</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>18042.599999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>2</v>
       </c>
@@ -5816,14 +5816,14 @@
         <v>17643.900000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>1</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>18052.3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>2</v>
       </c>
@@ -5857,14 +5857,14 @@
         <v>17722</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>1</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>17905.3</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>2</v>
       </c>
@@ -5898,14 +5898,14 @@
         <v>17717.400000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>1</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>18700.400000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>2</v>
       </c>
@@ -5939,14 +5939,14 @@
         <v>16962.3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>1</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>18159.3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>2</v>
       </c>
@@ -5980,14 +5980,14 @@
         <v>17220.099999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>1</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>17936.8</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>2</v>
       </c>
@@ -6021,14 +6021,14 @@
         <v>17609.8</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="6"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>1</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>18318</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>2</v>
       </c>
@@ -6062,14 +6062,14 @@
         <v>17736</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>1</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>18037.900000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>2</v>
       </c>
@@ -6103,14 +6103,14 @@
         <v>17696</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
       <c r="E119" s="6"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>1</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>18027.3</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>2</v>
       </c>
@@ -6144,8 +6144,8 @@
         <v>16868.099999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>1</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>17953.885000000002</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>2</v>
       </c>
@@ -6183,14 +6183,14 @@
         <v>17955.3</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="6"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>1</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>18279.5</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>2</v>
       </c>
@@ -6224,14 +6224,14 @@
         <v>17953.900000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="6"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>1</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>18101.3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>2</v>
       </c>
@@ -6265,14 +6265,14 @@
         <v>17671.2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="6"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>1</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>18024.400000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>2</v>
       </c>
@@ -6306,14 +6306,14 @@
         <v>17778.2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
       <c r="E134" s="6"/>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>1</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>18056</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>2</v>
       </c>
@@ -6347,14 +6347,14 @@
         <v>17356.900000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="6"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>1</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>17955.3</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>2</v>
       </c>
@@ -6388,14 +6388,14 @@
         <v>17620.900000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
       <c r="E140" s="6"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>1</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>18317.900000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>2</v>
       </c>
@@ -6429,14 +6429,14 @@
         <v>17630.7</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
       <c r="E143" s="6"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>1</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>18051.5</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>2</v>
       </c>
@@ -6470,14 +6470,14 @@
         <v>17955.400000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="6"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>1</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>17928.5</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>2</v>
       </c>
@@ -6511,14 +6511,14 @@
         <v>17684.599999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
       <c r="E149" s="6"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>1</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>18050.7</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
         <v>2</v>
       </c>
@@ -6552,8 +6552,8 @@
         <v>17627.2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>1</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>6885.54</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>2</v>
       </c>
@@ -6587,14 +6587,14 @@
         <v>6634.49</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
       <c r="E155" s="6"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>1</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>7114.61</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>2</v>
       </c>
@@ -6628,14 +6628,14 @@
         <v>6776.07</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
       <c r="E158" s="6"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>1</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>6922.12</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>2</v>
       </c>
@@ -6669,14 +6669,14 @@
         <v>6630.84</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
       <c r="E161" s="6"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>1</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>6937.99</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>2</v>
       </c>
@@ -6710,14 +6710,14 @@
         <v>6657.36</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
       <c r="E164" s="6"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>1</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>7025.04</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>2</v>
       </c>
@@ -6751,14 +6751,14 @@
         <v>6855.78</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
       <c r="E167" s="6"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>1</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>6971.51</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>2</v>
       </c>
@@ -6792,14 +6792,14 @@
         <v>6728.79</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
       <c r="E170" s="6"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>1</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>6908.98</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>2</v>
       </c>
@@ -6833,14 +6833,14 @@
         <v>6622.89</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
       <c r="E173" s="6"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>1</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>6963.14</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>2</v>
       </c>
@@ -6874,14 +6874,14 @@
         <v>6652.56</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
       <c r="E176" s="6"/>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>1</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>6943.32</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>2</v>
       </c>
@@ -6915,14 +6915,14 @@
         <v>6790.63</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
       <c r="E179" s="6"/>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>1</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>6953.72</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
         <v>2</v>
       </c>
@@ -6956,8 +6956,8 @@
         <v>6763.19</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>1</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>1000.35</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>2</v>
       </c>
@@ -6991,14 +6991,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
       <c r="E185" s="6"/>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>1</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>2</v>
       </c>
@@ -7032,14 +7032,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
       <c r="E188" s="6"/>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>1</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>1000.35</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>2</v>
       </c>
@@ -7073,14 +7073,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
       <c r="E191" s="6"/>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>1</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>2</v>
       </c>
@@ -7114,14 +7114,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
       <c r="E194" s="6"/>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>1</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>2</v>
       </c>
@@ -7155,14 +7155,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
       <c r="E197" s="6"/>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>1</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>2</v>
       </c>
@@ -7196,14 +7196,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
       <c r="E200" s="6"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>1</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>1000.4</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>2</v>
       </c>
@@ -7237,14 +7237,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
       <c r="E203" s="6"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>1</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>1000.4</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>2</v>
       </c>
@@ -7278,14 +7278,14 @@
         <v>1000.1</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
       <c r="D206" s="5"/>
       <c r="E206" s="6"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>1</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>1000.5</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>2</v>
       </c>
@@ -7319,14 +7319,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
       <c r="E209" s="6"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>1</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="7" t="s">
         <v>2</v>
       </c>
@@ -7360,8 +7360,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>1</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>2</v>
       </c>
@@ -7395,14 +7395,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
       <c r="E215" s="6"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>1</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>2</v>
       </c>
@@ -7436,14 +7436,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
       <c r="D218" s="5"/>
       <c r="E218" s="6"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>1</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>2</v>
       </c>
@@ -7477,14 +7477,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
       <c r="D221" s="5"/>
       <c r="E221" s="6"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>1</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>2</v>
       </c>
@@ -7518,14 +7518,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
       <c r="E224" s="6"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>1</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>2</v>
       </c>
@@ -7559,14 +7559,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
       <c r="C227" s="5"/>
       <c r="D227" s="5"/>
       <c r="E227" s="6"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
         <v>1</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>2</v>
       </c>
@@ -7600,14 +7600,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
       <c r="D230" s="5"/>
       <c r="E230" s="6"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>1</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
         <v>2</v>
       </c>
@@ -7641,14 +7641,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
       <c r="C233" s="5"/>
       <c r="D233" s="5"/>
       <c r="E233" s="6"/>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
         <v>1</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>2</v>
       </c>
@@ -7682,14 +7682,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
       <c r="D236" s="5"/>
       <c r="E236" s="6"/>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>1</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>2</v>
       </c>
@@ -7723,14 +7723,14 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
       <c r="D239" s="5"/>
       <c r="E239" s="6"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>1</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>1000.3</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="7" t="s">
         <v>2</v>
       </c>
@@ -7764,8 +7764,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="248" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="248" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="13" t="s">
         <v>9</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="10">
         <v>1</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>21543.599999999999</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="10">
         <v>1</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>19805.099999999999</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="10">
         <v>1</v>
       </c>
@@ -7869,7 +7869,7 @@
         <v>18554.7</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="10">
         <v>1</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>19539.7</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="10">
         <v>1</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>19505.8</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="10">
         <v>1</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>19927</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="10">
         <v>1</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>19987.8</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="10">
         <v>1</v>
       </c>
@@ -7999,7 +7999,7 @@
         <v>19770.3</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="10">
         <v>1</v>
       </c>
@@ -8025,7 +8025,7 @@
         <v>20378</v>
       </c>
     </row>
-    <row r="258" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="10">
         <v>1</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>19708.599999999999</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D259">
         <f>AVERAGE(D249:D258)</f>
         <v>19918.780000000002</v>
@@ -8065,8 +8065,8 @@
         <v>19895.419999999998</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="262" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="262" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="13" t="s">
         <v>9</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="263" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="10">
         <v>2</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>15105.1</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="10">
         <v>2</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>15200.6</v>
       </c>
     </row>
-    <row r="265" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="10">
         <v>2</v>
       </c>
@@ -8170,7 +8170,7 @@
         <v>14888.7</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="10">
         <v>2</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>15046.5</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="10">
         <v>2</v>
       </c>
@@ -8222,7 +8222,7 @@
         <v>15235.4</v>
       </c>
     </row>
-    <row r="268" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="10">
         <v>2</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>14625</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="10">
         <v>2</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>14827.2</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="10">
         <v>2</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>15114.7</v>
       </c>
     </row>
-    <row r="271" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="10">
         <v>2</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>15199.3</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="10">
         <v>2</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>14786.5</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D273">
         <f>AVERAGE(D263:D272)</f>
         <v>15564.009999999998</v>
@@ -8366,8 +8366,8 @@
         <v>15106.599999999999</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="278" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="278" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="13" t="s">
         <v>9</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="10">
         <v>3</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>10719.1</v>
       </c>
     </row>
-    <row r="280" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="10">
         <v>3</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>10700.4</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="10">
         <v>3</v>
       </c>
@@ -8471,7 +8471,7 @@
         <v>10579.1</v>
       </c>
     </row>
-    <row r="282" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="10">
         <v>3</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>10513.7</v>
       </c>
     </row>
-    <row r="283" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="10">
         <v>3</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>10458.4</v>
       </c>
     </row>
-    <row r="284" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="10">
         <v>3</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>10558.7</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="10">
         <v>3</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>10549.4</v>
       </c>
     </row>
-    <row r="286" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="10">
         <v>3</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>10497.6</v>
       </c>
     </row>
-    <row r="287" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="10">
         <v>3</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>10751.4</v>
       </c>
     </row>
-    <row r="288" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="10">
         <v>3</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>10339.299999999999</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D289">
         <f>AVERAGE(D279:D288)</f>
         <v>10948.570000000003</v>
@@ -8667,8 +8667,8 @@
         <v>10757.640000000003</v>
       </c>
     </row>
-    <row r="294" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="295" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="295" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="13" t="s">
         <v>9</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="10">
         <v>2</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>17801.400000000001</v>
       </c>
     </row>
-    <row r="297" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="10">
         <v>2</v>
       </c>
@@ -8746,7 +8746,7 @@
         <v>17643.900000000001</v>
       </c>
     </row>
-    <row r="298" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="10">
         <v>2</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>17722</v>
       </c>
     </row>
-    <row r="299" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="10">
         <v>2</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>17717.400000000001</v>
       </c>
     </row>
-    <row r="300" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="10">
         <v>2</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>16962.3</v>
       </c>
     </row>
-    <row r="301" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="10">
         <v>2</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>17220.099999999999</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="10">
         <v>2</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>17609.8</v>
       </c>
     </row>
-    <row r="303" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="10">
         <v>2</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>17736</v>
       </c>
     </row>
-    <row r="304" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="10">
         <v>2</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>17696</v>
       </c>
     </row>
-    <row r="305" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="10">
         <v>2</v>
       </c>
@@ -8954,7 +8954,7 @@
         <v>16868.099999999999</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D306">
         <f>AVERAGE(D296:D305)</f>
         <v>18125.96</v>
@@ -8968,8 +8968,8 @@
         <v>17811.830000000002</v>
       </c>
     </row>
-    <row r="311" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="312" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="312" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="13" t="s">
         <v>9</v>
       </c>
@@ -8995,7 +8995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="313" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="10">
         <v>1</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>17955.3</v>
       </c>
     </row>
-    <row r="314" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="10">
         <v>1</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>17953.900000000001</v>
       </c>
     </row>
-    <row r="315" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="10">
         <v>1</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>17671.2</v>
       </c>
     </row>
-    <row r="316" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="10">
         <v>1</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>17778.2</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="10">
         <v>1</v>
       </c>
@@ -9125,7 +9125,7 @@
         <v>17356.900000000001</v>
       </c>
     </row>
-    <row r="318" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="10">
         <v>1</v>
       </c>
@@ -9151,7 +9151,7 @@
         <v>17620.900000000001</v>
       </c>
     </row>
-    <row r="319" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="10">
         <v>1</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v>17630.7</v>
       </c>
     </row>
-    <row r="320" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="10">
         <v>1</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>17955.400000000001</v>
       </c>
     </row>
-    <row r="321" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="10">
         <v>1</v>
       </c>
@@ -9229,7 +9229,7 @@
         <v>17684.599999999999</v>
       </c>
     </row>
-    <row r="322" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="10">
         <v>1</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>17627.2</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D323">
         <f>AVERAGE(D313:D322)</f>
         <v>18184.340000000004</v>
@@ -9269,8 +9269,8 @@
         <v>17953.885000000002</v>
       </c>
     </row>
-    <row r="327" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="328" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="328" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="13" t="s">
         <v>9</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="329" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="10">
         <v>1</v>
       </c>
@@ -9322,7 +9322,7 @@
         <v>15094.7</v>
       </c>
     </row>
-    <row r="330" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="10">
         <v>1</v>
       </c>
@@ -9348,7 +9348,7 @@
         <v>15114.5</v>
       </c>
     </row>
-    <row r="331" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="10">
         <v>1</v>
       </c>
@@ -9374,7 +9374,7 @@
         <v>15444.4</v>
       </c>
     </row>
-    <row r="332" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="10">
         <v>1</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>15137.8</v>
       </c>
     </row>
-    <row r="333" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="10">
         <v>1</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>15324.2</v>
       </c>
     </row>
-    <row r="334" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="10">
         <v>1</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>15135.5</v>
       </c>
     </row>
-    <row r="335" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="10">
         <v>1</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>15026.6</v>
       </c>
     </row>
-    <row r="336" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="10">
         <v>1</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>15332.7</v>
       </c>
     </row>
-    <row r="337" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="10">
         <v>1</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>15224.4</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" s="10">
         <v>1</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>15255.6</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D339">
         <f>AVERAGE(D329:D338)</f>
         <v>15657.73</v>
@@ -9570,8 +9570,8 @@
         <v>15433.384999999998</v>
       </c>
     </row>
-    <row r="341" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="342" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="342" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" s="13" t="s">
         <v>9</v>
       </c>
@@ -9597,7 +9597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="343" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" s="10">
         <v>3</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>14402.5</v>
       </c>
     </row>
-    <row r="344" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" s="10">
         <v>3</v>
       </c>
@@ -9649,7 +9649,7 @@
         <v>14713.6</v>
       </c>
     </row>
-    <row r="345" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="10">
         <v>3</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>15041.7</v>
       </c>
     </row>
-    <row r="346" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" s="10">
         <v>3</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>14771</v>
       </c>
     </row>
-    <row r="347" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="10">
         <v>3</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>14714.3</v>
       </c>
     </row>
-    <row r="348" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" s="10">
         <v>3</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>14833</v>
       </c>
     </row>
-    <row r="349" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="10">
         <v>3</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>15071.9</v>
       </c>
     </row>
-    <row r="350" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" s="10">
         <v>3</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>14669.9</v>
       </c>
     </row>
-    <row r="351" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" s="10">
         <v>3</v>
       </c>
@@ -9831,7 +9831,7 @@
         <v>15391</v>
       </c>
     </row>
-    <row r="352" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="10">
         <v>3</v>
       </c>
@@ -9857,7 +9857,7 @@
         <v>15362.8</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D353">
         <f>AVERAGE(D343:D352)</f>
         <v>15385.829999999998</v>
@@ -9871,8 +9871,8 @@
         <v>15141.499999999998</v>
       </c>
     </row>
-    <row r="357" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="358" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="358" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358" s="13" t="s">
         <v>9</v>
       </c>
@@ -9898,7 +9898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="359" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="10">
         <v>5</v>
       </c>
@@ -9924,7 +9924,7 @@
         <v>6634.49</v>
       </c>
     </row>
-    <row r="360" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="10">
         <v>5</v>
       </c>
@@ -9950,7 +9950,7 @@
         <v>6776.07</v>
       </c>
     </row>
-    <row r="361" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="10">
         <v>5</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>6630.84</v>
       </c>
     </row>
-    <row r="362" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362" s="10">
         <v>5</v>
       </c>
@@ -10002,7 +10002,7 @@
         <v>6657.36</v>
       </c>
     </row>
-    <row r="363" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363" s="10">
         <v>5</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>6855.78</v>
       </c>
     </row>
-    <row r="364" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="10">
         <v>5</v>
       </c>
@@ -10054,7 +10054,7 @@
         <v>6728.79</v>
       </c>
     </row>
-    <row r="365" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="10">
         <v>5</v>
       </c>
@@ -10080,7 +10080,7 @@
         <v>6622.89</v>
       </c>
     </row>
-    <row r="366" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="10">
         <v>5</v>
       </c>
@@ -10106,7 +10106,7 @@
         <v>6652.56</v>
       </c>
     </row>
-    <row r="367" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367" s="10">
         <v>5</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>6790.63</v>
       </c>
     </row>
-    <row r="368" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368" s="10">
         <v>5</v>
       </c>
@@ -10158,7 +10158,7 @@
         <v>6763.19</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D369">
         <f>AVERAGE(D359:D368)</f>
         <v>6962.5969999999998</v>
@@ -10172,7 +10172,7 @@
         <v>6836.9285</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A373" s="17" t="s">
         <v>17</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A374" s="17">
         <v>1</v>
       </c>
@@ -10230,7 +10230,7 @@
         <v>19872.060000000001</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A375" s="17">
         <v>2</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>15002.9</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A376" s="17">
         <v>3</v>
       </c>
@@ -10288,7 +10288,7 @@
         <v>10566.17</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A377" s="17">
         <v>1</v>
       </c>
@@ -10317,7 +10317,7 @@
         <v>17497.7</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A378" s="17">
         <v>2</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>17723.43</v>
       </c>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A379" s="17">
         <v>1</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>14897.17</v>
       </c>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A380" s="17">
         <v>3</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>15209.04</v>
       </c>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A381" s="17">
         <v>5</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>6711.26</v>
       </c>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B385" s="17" t="s">
         <v>19</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B386" s="17">
         <v>2</v>
       </c>
@@ -10449,7 +10449,7 @@
         <v>19895.419999999998</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B387" s="17">
         <v>4</v>
       </c>
@@ -10457,7 +10457,7 @@
         <v>15106.6</v>
       </c>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B388" s="17">
         <v>6</v>
       </c>
@@ -10465,7 +10465,7 @@
         <v>10757.64</v>
       </c>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B389" s="17">
         <v>3</v>
       </c>
@@ -10473,7 +10473,7 @@
         <v>17953.89</v>
       </c>
     </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B390" s="17">
         <v>3</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>17811.830000000002</v>
       </c>
     </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B391" s="17">
         <v>4</v>
       </c>
@@ -10489,7 +10489,7 @@
         <v>15433.39</v>
       </c>
     </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B392" s="17">
         <v>4</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>15141.5</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B393" s="17">
         <v>10</v>
       </c>
@@ -10505,8 +10505,8 @@
         <v>6836.9290000000001</v>
       </c>
     </row>
-    <row r="412" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="413" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="412" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="413" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C413" s="19">
         <v>9618.02</v>
       </c>
@@ -10514,7 +10514,7 @@
         <v>9342.2000000000007</v>
       </c>
     </row>
-    <row r="414" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="414" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C414" s="20">
         <v>8601</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>8974.76</v>
       </c>
     </row>
-    <row r="415" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="415" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C415" s="20">
         <v>9003.2000000000007</v>
       </c>
@@ -10530,7 +10530,7 @@
         <v>8845.6200000000008</v>
       </c>
     </row>
-    <row r="416" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="416" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C416" s="20">
         <v>8836.1299999999992</v>
       </c>
@@ -10538,7 +10538,7 @@
         <v>8593.48</v>
       </c>
     </row>
-    <row r="417" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="417" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C417" s="20">
         <v>8785.83</v>
       </c>
@@ -10546,7 +10546,7 @@
         <v>8449.67</v>
       </c>
     </row>
-    <row r="418" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="418" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C418" s="20">
         <v>8963.23</v>
       </c>
@@ -10554,7 +10554,7 @@
         <v>9032.8700000000008</v>
       </c>
     </row>
-    <row r="419" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="419" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C419" s="20">
         <v>9629.0300000000007</v>
       </c>
@@ -10562,7 +10562,7 @@
         <v>9507.6200000000008</v>
       </c>
     </row>
-    <row r="420" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="420" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C420" s="20">
         <v>9048.23</v>
       </c>
@@ -10570,7 +10570,7 @@
         <v>8358.2199999999993</v>
       </c>
     </row>
-    <row r="421" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="421" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C421" s="20">
         <v>8501.49</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>8136.17</v>
       </c>
     </row>
-    <row r="422" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="422" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C422" s="20">
         <v>9220.7900000000009</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>8752.65</v>
       </c>
     </row>
-    <row r="424" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="424" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C424">
         <f>AVERAGE(C413:C422)</f>
         <v>9020.6950000000015</v>
@@ -10596,7 +10596,7 @@
         <v>8799.3259999999991</v>
       </c>
     </row>
-    <row r="427" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D427">
         <f>AVERAGE(C424:E424)</f>
         <v>8910.0105000000003</v>

</xml_diff>